<commit_message>
corr analysis and updated data dictionary with correlation
</commit_message>
<xml_diff>
--- a/data/zillow_data_dictionary.xlsx
+++ b/data/zillow_data_dictionary.xlsx
@@ -1,46 +1,59 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26915"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10313"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binhe/zdabh/kaggle/published_to_kaggle/kaggle_publish_history/2017-05-04/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathanbugg/Desktop/lin_reg_proj/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5791E134-E3CA-9748-90BD-CC829F8BC7EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16900" yWindow="-20780" windowWidth="27600" windowHeight="15880"/>
+    <workbookView xWindow="280" yWindow="800" windowWidth="26840" windowHeight="17300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Dictionary" sheetId="5" r:id="rId1"/>
-    <sheet name="HeatingOrSystemTypeID" sheetId="6" r:id="rId2"/>
-    <sheet name="PropertyLandUseTypeID" sheetId="7" r:id="rId3"/>
-    <sheet name="StoryTypeID" sheetId="1" r:id="rId4"/>
-    <sheet name="AirConditioningTypeID" sheetId="2" r:id="rId5"/>
-    <sheet name="ArchitecturalStyleTypeID" sheetId="3" r:id="rId6"/>
-    <sheet name="TypeConstructionTypeID" sheetId="4" r:id="rId7"/>
-    <sheet name="BuildingClassTypeID" sheetId="9" r:id="rId8"/>
+    <sheet name="multi-col" sheetId="11" r:id="rId2"/>
+    <sheet name="HeatingOrSystemTypeID" sheetId="6" r:id="rId3"/>
+    <sheet name="PropertyLandUseTypeID" sheetId="7" r:id="rId4"/>
+    <sheet name="StoryTypeID" sheetId="1" r:id="rId5"/>
+    <sheet name="AirConditioningTypeID" sheetId="2" r:id="rId6"/>
+    <sheet name="ArchitecturalStyleTypeID" sheetId="3" r:id="rId7"/>
+    <sheet name="TypeConstructionTypeID" sheetId="4" r:id="rId8"/>
+    <sheet name="BuildingClassTypeID" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">PropertyLandUseTypeID!$A$1:$B$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Data Dictionary'!$A$1:$F$59</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">PropertyLandUseTypeID!$A$1:$B$26</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="293">
   <si>
     <t>StoryTypeID</t>
   </si>
@@ -708,9 +721,6 @@
     <t>'finishedfloor1squarefeet'</t>
   </si>
   <si>
-    <t>'calculatedfinishedsquarefeet'</t>
-  </si>
-  <si>
     <t>'finishedsquarefeet6'</t>
   </si>
   <si>
@@ -844,19 +854,118 @@
   </si>
   <si>
     <t>'taxdelinquencyflag'</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Categorical</t>
+  </si>
+  <si>
+    <t>Numeric</t>
+  </si>
+  <si>
+    <t>Ordinal</t>
+  </si>
+  <si>
+    <t>N/a</t>
+  </si>
+  <si>
+    <t>Na Handling</t>
+  </si>
+  <si>
+    <t>Multicol Considerations</t>
+  </si>
+  <si>
+    <t>bathroomcnt</t>
+  </si>
+  <si>
+    <t>bedroomcnt</t>
+  </si>
+  <si>
+    <t>calculatedbathnbr</t>
+  </si>
+  <si>
+    <t>finishedfloor1squarefeet</t>
+  </si>
+  <si>
+    <t>calculatedfinishedsquarefeet</t>
+  </si>
+  <si>
+    <t>finishedsquarefeet12</t>
+  </si>
+  <si>
+    <t>fullbathcnt</t>
+  </si>
+  <si>
+    <t>garagecarcnt</t>
+  </si>
+  <si>
+    <t>garagetotalsqft</t>
+  </si>
+  <si>
+    <t>threequarterbathnbr</t>
+  </si>
+  <si>
+    <t>yearbuilt</t>
+  </si>
+  <si>
+    <t>structuretaxvaluedollarcnt</t>
+  </si>
+  <si>
+    <t>taxamount</t>
+  </si>
+  <si>
+    <t>NaN</t>
+  </si>
+  <si>
+    <t>calculatedfinishedsquarefeet'</t>
+  </si>
+  <si>
+    <t>Drop if use calculatedfinishedsquarefeet</t>
+  </si>
+  <si>
+    <t>Drop if use calculatedbathnbr</t>
+  </si>
+  <si>
+    <t>Drop if use taxamount</t>
+  </si>
+  <si>
+    <t>Set zero if NA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -879,13 +988,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1160,489 +1284,1832 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B59"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" zoomScale="165" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="41.6640625" customWidth="1"/>
-    <col min="2" max="2" width="55.33203125" customWidth="1"/>
+    <col min="1" max="1" width="20.5" customWidth="1"/>
+    <col min="2" max="2" width="64.1640625" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.33203125" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" t="s">
+        <v>268</v>
+      </c>
+      <c r="D2" t="s">
+        <v>292</v>
+      </c>
+      <c r="F2" t="str">
+        <f>_xlfn.CONCAT(A2, " :  ", "'",C2,"',")</f>
+        <v>'airconditioningtypeid' :  'Categorical',</v>
+      </c>
+      <c r="K2" s="2"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>212</v>
+      </c>
+      <c r="B3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C3" t="s">
+        <v>268</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F59" si="0">_xlfn.CONCAT(A3, " :  ", "'",C3,"',")</f>
+        <v>'architecturalstyletypeid' :  'Categorical',</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>213</v>
+      </c>
+      <c r="B4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" t="s">
+        <v>269</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>'basementsqft' :  'Numeric',</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>214</v>
+      </c>
+      <c r="B5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" t="s">
+        <v>269</v>
+      </c>
+      <c r="E5" t="s">
+        <v>290</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>'bathroomcnt' :  'Numeric',</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>215</v>
+      </c>
+      <c r="B6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C6" t="s">
+        <v>269</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>'bedroomcnt' :  'Numeric',</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>216</v>
+      </c>
+      <c r="B7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7" t="s">
+        <v>270</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>'buildingqualitytypeid' :  'Ordinal',</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>217</v>
+      </c>
+      <c r="B8" t="s">
+        <v>206</v>
+      </c>
+      <c r="C8" t="s">
+        <v>268</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>'buildingclasstypeid' :  'Categorical',</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>218</v>
+      </c>
+      <c r="B9" t="s">
+        <v>102</v>
+      </c>
+      <c r="C9" t="s">
+        <v>269</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>'calculatedbathnbr' :  'Numeric',</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>219</v>
+      </c>
+      <c r="B10" t="s">
+        <v>179</v>
+      </c>
+      <c r="C10" t="s">
+        <v>268</v>
+      </c>
+      <c r="D10" t="s">
+        <v>292</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>'decktypeid' :  'Categorical',</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>220</v>
+      </c>
+      <c r="B11" t="s">
+        <v>103</v>
+      </c>
+      <c r="C11" t="s">
+        <v>269</v>
+      </c>
+      <c r="E11" t="s">
+        <v>290</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>'threequarterbathnbr' :  'Numeric',</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>221</v>
+      </c>
+      <c r="B12" t="s">
+        <v>104</v>
+      </c>
+      <c r="C12" t="s">
+        <v>269</v>
+      </c>
+      <c r="E12" t="s">
+        <v>289</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>'finishedfloor1squarefeet' :  'Numeric',</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="B13" t="s">
+        <v>203</v>
+      </c>
+      <c r="C13" t="s">
+        <v>269</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>calculatedfinishedsquarefeet' :  'Numeric',</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>222</v>
+      </c>
+      <c r="B14" t="s">
+        <v>202</v>
+      </c>
+      <c r="C14" t="s">
+        <v>269</v>
+      </c>
+      <c r="E14" t="s">
+        <v>289</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
+        <v>'finishedsquarefeet6' :  'Numeric',</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>223</v>
+      </c>
+      <c r="B15" t="s">
+        <v>207</v>
+      </c>
+      <c r="C15" t="s">
+        <v>269</v>
+      </c>
+      <c r="E15" t="s">
+        <v>289</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="0"/>
+        <v>'finishedsquarefeet12' :  'Numeric',</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>224</v>
+      </c>
+      <c r="B16" t="s">
+        <v>208</v>
+      </c>
+      <c r="C16" t="s">
+        <v>269</v>
+      </c>
+      <c r="E16" t="s">
+        <v>289</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="0"/>
+        <v>'finishedsquarefeet13' :  'Numeric',</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>225</v>
+      </c>
+      <c r="B17" t="s">
+        <v>209</v>
+      </c>
+      <c r="C17" t="s">
+        <v>269</v>
+      </c>
+      <c r="E17" t="s">
+        <v>289</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="0"/>
+        <v>'finishedsquarefeet15' :  'Numeric',</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>226</v>
+      </c>
+      <c r="B18" t="s">
+        <v>104</v>
+      </c>
+      <c r="C18" t="s">
+        <v>269</v>
+      </c>
+      <c r="E18" t="s">
+        <v>289</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="0"/>
+        <v>'finishedsquarefeet50' :  'Numeric',</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>227</v>
+      </c>
+      <c r="B19" t="s">
+        <v>183</v>
+      </c>
+      <c r="C19" t="s">
+        <v>271</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="0"/>
+        <v>'fips' :  'N/a',</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>228</v>
+      </c>
+      <c r="B20" t="s">
+        <v>105</v>
+      </c>
+      <c r="C20" t="s">
+        <v>270</v>
+      </c>
+      <c r="D20" t="s">
+        <v>292</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="0"/>
+        <v>'fireplacecnt' :  'Ordinal',</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>229</v>
+      </c>
+      <c r="B21" t="s">
+        <v>189</v>
+      </c>
+      <c r="C21" t="s">
+        <v>268</v>
+      </c>
+      <c r="D21" t="s">
+        <v>292</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="0"/>
+        <v>'fireplaceflag' :  'Categorical',</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>230</v>
+      </c>
+      <c r="B22" t="s">
+        <v>106</v>
+      </c>
+      <c r="C22" t="s">
+        <v>269</v>
+      </c>
+      <c r="E22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" si="0"/>
+        <v>'fullbathcnt' :  'Numeric',</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>231</v>
+      </c>
+      <c r="B23" t="s">
+        <v>107</v>
+      </c>
+      <c r="C23" t="s">
+        <v>269</v>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" si="0"/>
+        <v>'garagecarcnt' :  'Numeric',</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>232</v>
+      </c>
+      <c r="B24" t="s">
+        <v>186</v>
+      </c>
+      <c r="C24" t="s">
+        <v>269</v>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" si="0"/>
+        <v>'garagetotalsqft' :  'Numeric',</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>233</v>
+      </c>
+      <c r="B25" t="s">
+        <v>185</v>
+      </c>
+      <c r="C25" t="s">
+        <v>268</v>
+      </c>
+      <c r="F25" t="str">
+        <f t="shared" si="0"/>
+        <v>'hashottuborspa' :  'Categorical',</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>234</v>
+      </c>
+      <c r="B26" t="s">
+        <v>108</v>
+      </c>
+      <c r="C26" t="s">
+        <v>268</v>
+      </c>
+      <c r="F26" t="str">
+        <f t="shared" si="0"/>
+        <v>'heatingorsystemtypeid' :  'Categorical',</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>235</v>
+      </c>
+      <c r="B27" t="s">
+        <v>109</v>
+      </c>
+      <c r="C27" t="s">
+        <v>271</v>
+      </c>
+      <c r="F27" t="str">
+        <f t="shared" si="0"/>
+        <v>'latitude' :  'N/a',</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>236</v>
+      </c>
+      <c r="B28" t="s">
+        <v>190</v>
+      </c>
+      <c r="C28" t="s">
+        <v>271</v>
+      </c>
+      <c r="F28" t="str">
+        <f t="shared" si="0"/>
+        <v>'longitude' :  'N/a',</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>237</v>
+      </c>
+      <c r="B29" t="s">
+        <v>187</v>
+      </c>
+      <c r="C29" t="s">
+        <v>269</v>
+      </c>
+      <c r="F29" t="str">
+        <f t="shared" si="0"/>
+        <v>'lotsizesquarefeet' :  'Numeric',</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>238</v>
+      </c>
+      <c r="B30" t="s">
+        <v>110</v>
+      </c>
+      <c r="C30" t="s">
+        <v>270</v>
+      </c>
+      <c r="F30" t="str">
+        <f t="shared" si="0"/>
+        <v>'numberofstories' :  'Ordinal',</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>239</v>
+      </c>
+      <c r="B31" t="s">
+        <v>111</v>
+      </c>
+      <c r="C31" t="s">
+        <v>271</v>
+      </c>
+      <c r="F31" t="str">
+        <f t="shared" si="0"/>
+        <v>'parcelid' :  'N/a',</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>240</v>
+      </c>
+      <c r="B32" t="s">
+        <v>112</v>
+      </c>
+      <c r="C32" t="s">
+        <v>268</v>
+      </c>
+      <c r="F32" t="str">
+        <f t="shared" si="0"/>
+        <v>'poolcnt' :  'Categorical',</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>241</v>
+      </c>
+      <c r="B33" t="s">
+        <v>113</v>
+      </c>
+      <c r="C33" t="s">
+        <v>269</v>
+      </c>
+      <c r="F33" t="str">
+        <f t="shared" si="0"/>
+        <v>'poolsizesum' :  'Numeric',</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>242</v>
+      </c>
+      <c r="B34" t="s">
+        <v>114</v>
+      </c>
+      <c r="C34" t="s">
+        <v>268</v>
+      </c>
+      <c r="F34" t="str">
+        <f t="shared" si="0"/>
+        <v>'pooltypeid10' :  'Categorical',</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>243</v>
+      </c>
+      <c r="B35" t="s">
+        <v>115</v>
+      </c>
+      <c r="C35" t="s">
+        <v>268</v>
+      </c>
+      <c r="F35" t="str">
+        <f t="shared" si="0"/>
+        <v>'pooltypeid2' :  'Categorical',</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>244</v>
+      </c>
+      <c r="B36" t="s">
+        <v>116</v>
+      </c>
+      <c r="C36" t="s">
+        <v>268</v>
+      </c>
+      <c r="F36" t="str">
+        <f t="shared" si="0"/>
+        <v>'pooltypeid7' :  'Categorical',</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>245</v>
+      </c>
+      <c r="B37" t="s">
+        <v>117</v>
+      </c>
+      <c r="C37" t="s">
+        <v>271</v>
+      </c>
+      <c r="F37" t="str">
+        <f t="shared" si="0"/>
+        <v>'propertycountylandusecode' :  'N/a',</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>246</v>
+      </c>
+      <c r="B38" t="s">
+        <v>118</v>
+      </c>
+      <c r="C38" t="s">
+        <v>268</v>
+      </c>
+      <c r="F38" t="str">
+        <f t="shared" si="0"/>
+        <v>'propertylandusetypeid' :  'Categorical',</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>247</v>
+      </c>
+      <c r="B39" t="s">
+        <v>119</v>
+      </c>
+      <c r="C39" t="s">
+        <v>268</v>
+      </c>
+      <c r="F39" t="str">
+        <f t="shared" si="0"/>
+        <v>'propertyzoningdesc' :  'Categorical',</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>248</v>
+      </c>
+      <c r="B40" t="s">
+        <v>188</v>
+      </c>
+      <c r="C40" t="s">
+        <v>271</v>
+      </c>
+      <c r="F40" t="str">
+        <f t="shared" si="0"/>
+        <v>'rawcensustractandblock' :  'N/a',</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>249</v>
+      </c>
+      <c r="B41" t="s">
+        <v>188</v>
+      </c>
+      <c r="C41" t="s">
+        <v>271</v>
+      </c>
+      <c r="F41" t="str">
+        <f t="shared" si="0"/>
+        <v>'censustractandblock' :  'N/a',</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>250</v>
+      </c>
+      <c r="B42" t="s">
+        <v>180</v>
+      </c>
+      <c r="C42" t="s">
+        <v>268</v>
+      </c>
+      <c r="F42" t="str">
+        <f t="shared" si="0"/>
+        <v>'regionidcounty' :  'Categorical',</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>251</v>
+      </c>
+      <c r="B43" t="s">
+        <v>120</v>
+      </c>
+      <c r="C43" t="s">
+        <v>268</v>
+      </c>
+      <c r="F43" t="str">
+        <f t="shared" si="0"/>
+        <v>'regionidcity' :  'Categorical',</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>252</v>
+      </c>
+      <c r="B44" t="s">
+        <v>121</v>
+      </c>
+      <c r="C44" t="s">
+        <v>268</v>
+      </c>
+      <c r="F44" t="str">
+        <f t="shared" si="0"/>
+        <v>'regionidzip' :  'Categorical',</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>253</v>
+      </c>
+      <c r="B45" t="s">
+        <v>201</v>
+      </c>
+      <c r="C45" t="s">
+        <v>268</v>
+      </c>
+      <c r="F45" t="str">
+        <f t="shared" si="0"/>
+        <v>'regionidneighborhood' :  'Categorical',</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>254</v>
+      </c>
+      <c r="B46" t="s">
+        <v>122</v>
+      </c>
+      <c r="C46" t="s">
+        <v>269</v>
+      </c>
+      <c r="F46" t="str">
+        <f t="shared" si="0"/>
+        <v>'roomcnt' :  'Numeric',</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>255</v>
+      </c>
+      <c r="B47" t="s">
+        <v>184</v>
+      </c>
+      <c r="C47" t="s">
+        <v>268</v>
+      </c>
+      <c r="F47" t="str">
+        <f t="shared" si="0"/>
+        <v>'storytypeid' :  'Categorical',</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>256</v>
+      </c>
+      <c r="B48" t="s">
+        <v>181</v>
+      </c>
+      <c r="C48" t="s">
+        <v>268</v>
+      </c>
+      <c r="F48" t="str">
+        <f t="shared" si="0"/>
+        <v>'typeconstructiontypeid' :  'Categorical',</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>257</v>
+      </c>
+      <c r="B49" t="s">
+        <v>123</v>
+      </c>
+      <c r="C49" t="s">
+        <v>270</v>
+      </c>
+      <c r="F49" t="str">
+        <f t="shared" si="0"/>
+        <v>'unitcnt' :  'Ordinal',</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>258</v>
+      </c>
+      <c r="B50" t="s">
+        <v>127</v>
+      </c>
+      <c r="C50" t="s">
+        <v>269</v>
+      </c>
+      <c r="F50" t="str">
+        <f t="shared" si="0"/>
+        <v>'yardbuildingsqft17' :  'Numeric',</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>259</v>
+      </c>
+      <c r="B51" t="s">
+        <v>128</v>
+      </c>
+      <c r="C51" t="s">
+        <v>269</v>
+      </c>
+      <c r="F51" t="str">
+        <f t="shared" si="0"/>
+        <v>'yardbuildingsqft26' :  'Numeric',</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>260</v>
+      </c>
+      <c r="B52" t="s">
+        <v>124</v>
+      </c>
+      <c r="C52" t="s">
+        <v>269</v>
+      </c>
+      <c r="F52" t="str">
+        <f t="shared" si="0"/>
+        <v>'yearbuilt' :  'Numeric',</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>261</v>
+      </c>
+      <c r="B53" t="s">
+        <v>129</v>
+      </c>
+      <c r="C53" t="s">
+        <v>269</v>
+      </c>
+      <c r="E53" t="s">
+        <v>291</v>
+      </c>
+      <c r="F53" t="str">
+        <f t="shared" si="0"/>
+        <v>'taxvaluedollarcnt' :  'Numeric',</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>262</v>
+      </c>
+      <c r="B54" t="s">
+        <v>131</v>
+      </c>
+      <c r="C54" t="s">
+        <v>269</v>
+      </c>
+      <c r="E54" t="s">
+        <v>291</v>
+      </c>
+      <c r="F54" t="str">
+        <f t="shared" si="0"/>
+        <v>'structuretaxvaluedollarcnt' :  'Numeric',</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>263</v>
+      </c>
+      <c r="B55" t="s">
+        <v>130</v>
+      </c>
+      <c r="C55" t="s">
+        <v>269</v>
+      </c>
+      <c r="E55" t="s">
+        <v>291</v>
+      </c>
+      <c r="F55" t="str">
+        <f t="shared" si="0"/>
+        <v>'landtaxvaluedollarcnt' :  'Numeric',</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>264</v>
+      </c>
+      <c r="B56" t="s">
+        <v>192</v>
+      </c>
+      <c r="C56" t="s">
+        <v>269</v>
+      </c>
+      <c r="F56" t="str">
+        <f t="shared" si="0"/>
+        <v>'taxamount' :  'Numeric',</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>265</v>
+      </c>
+      <c r="B57" t="s">
+        <v>193</v>
+      </c>
+      <c r="C57" t="s">
+        <v>269</v>
+      </c>
+      <c r="F57" t="str">
+        <f t="shared" si="0"/>
+        <v>'assessmentyear' :  'Numeric',</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>266</v>
+      </c>
+      <c r="B58" t="s">
+        <v>204</v>
+      </c>
+      <c r="C58" t="s">
+        <v>268</v>
+      </c>
+      <c r="F58" t="str">
+        <f t="shared" si="0"/>
+        <v>'taxdelinquencyflag' :  'Categorical',</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>210</v>
+      </c>
+      <c r="B59" t="s">
+        <v>205</v>
+      </c>
+      <c r="C59" t="s">
+        <v>268</v>
+      </c>
+      <c r="F59" t="str">
+        <f t="shared" si="0"/>
+        <v>'taxdelinquencyyear' :  'Categorical',</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:F59" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Categorical"/>
+        <filter val="Numeric"/>
+        <filter val="Ordinal"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0BE19A5-57F5-0942-9DCD-96EB1609D9F4}">
+  <dimension ref="A1:N15"/>
+  <sheetViews>
+    <sheetView zoomScale="137" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.83203125" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" customWidth="1"/>
+    <col min="6" max="6" width="20.83203125" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="B1" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.64612000000000003</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0.47726400000000002</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0.77255300000000005</v>
+      </c>
+      <c r="G2" s="3">
+        <v>0.79937199999999997</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0.98412999999999995</v>
+      </c>
+      <c r="I2" s="3">
+        <v>0.50242900000000001</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0.45106200000000002</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0.26026300000000002</v>
+      </c>
+      <c r="L2" s="3">
+        <v>0.36806100000000003</v>
+      </c>
+      <c r="M2" s="3">
+        <v>0.58664099999999997</v>
+      </c>
+      <c r="N2" s="3">
+        <v>0.46189999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.64612000000000003</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.61806000000000005</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.45802999999999999</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.63203500000000001</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0.65759900000000004</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0.61375299999999999</v>
+      </c>
+      <c r="I3" s="3">
+        <v>0.43211500000000003</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0.59149600000000002</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0.11131199999999999</v>
+      </c>
+      <c r="L3" s="3">
+        <v>4.0870999999999998E-2</v>
+      </c>
+      <c r="M3" s="3">
+        <v>0.30540499999999998</v>
+      </c>
+      <c r="N3" s="3">
+        <v>0.239118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.61806000000000005</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.49180400000000002</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.80120800000000003</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0.80547500000000005</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0.98412999999999995</v>
+      </c>
+      <c r="I4" s="3">
+        <v>0.47986200000000001</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0.44441799999999998</v>
+      </c>
+      <c r="K4" s="3">
+        <v>0.26026300000000002</v>
+      </c>
+      <c r="L4" s="3">
+        <v>0.36954300000000001</v>
+      </c>
+      <c r="M4" s="3">
+        <v>0.61166500000000001</v>
+      </c>
+      <c r="N4" s="3">
+        <v>0.48731999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.47726400000000002</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.45802999999999999</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.49180400000000002</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.70352499999999996</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0.70359300000000002</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0.52914600000000001</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0.46176499999999998</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0.60377700000000001</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="L5" s="3">
+        <v>4.5581000000000003E-2</v>
+      </c>
+      <c r="M5" s="3">
+        <v>0.59738100000000005</v>
+      </c>
+      <c r="N5" s="3">
+        <v>0.51170800000000005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.77255300000000005</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.63203500000000001</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.80120800000000003</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.70352499999999996</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3">
+        <v>1</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0.78032500000000005</v>
+      </c>
+      <c r="I6" s="3">
+        <v>0.506166</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0.60436000000000001</v>
+      </c>
+      <c r="K6" s="3">
+        <v>0.32011299999999998</v>
+      </c>
+      <c r="L6" s="3">
+        <v>0.211641</v>
+      </c>
+      <c r="M6" s="3">
+        <v>0.71648900000000004</v>
+      </c>
+      <c r="N6" s="3">
+        <v>0.58902200000000005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.79937199999999997</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.65759900000000004</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.80547500000000005</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.70359300000000002</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3">
+        <v>1</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0.78295599999999999</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0.55305899999999997</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0.62593799999999999</v>
+      </c>
+      <c r="K7" s="3">
+        <v>0.31992999999999999</v>
+      </c>
+      <c r="L7" s="3">
+        <v>0.25852999999999998</v>
+      </c>
+      <c r="M7" s="3">
+        <v>0.74404800000000004</v>
+      </c>
+      <c r="N7" s="3">
+        <v>0.61249600000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.98412999999999995</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.61375299999999999</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.98412999999999995</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.52914600000000001</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0.78032500000000005</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0.78295599999999999</v>
+      </c>
+      <c r="H8" s="3">
+        <v>1</v>
+      </c>
+      <c r="I8" s="3">
+        <v>0.45486500000000002</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0.46444600000000003</v>
+      </c>
+      <c r="K8" s="3">
+        <v>0.20709</v>
+      </c>
+      <c r="L8" s="3">
+        <v>0.32253500000000002</v>
+      </c>
+      <c r="M8" s="3">
+        <v>0.59240999999999999</v>
+      </c>
+      <c r="N8" s="3">
+        <v>0.47600999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.50242900000000001</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.43211500000000003</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.47986200000000001</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.46176499999999998</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.506166</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0.55305899999999997</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0.45486500000000002</v>
+      </c>
+      <c r="I9" s="3">
+        <v>1</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0.64188299999999998</v>
+      </c>
+      <c r="K9" s="3">
+        <v>0.24285399999999999</v>
+      </c>
+      <c r="L9" s="3">
+        <v>0.19620899999999999</v>
+      </c>
+      <c r="M9" s="3">
+        <v>0.473109</v>
+      </c>
+      <c r="N9" s="3">
+        <v>0.35311399999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0.45106200000000002</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.59149600000000002</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.44441799999999998</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.60377700000000001</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0.60436000000000001</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0.62593799999999999</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0.46444600000000003</v>
+      </c>
+      <c r="I10" s="3">
+        <v>0.64188299999999998</v>
+      </c>
+      <c r="J10" s="3">
+        <v>1</v>
+      </c>
+      <c r="K10" s="3">
+        <v>0.19302</v>
+      </c>
+      <c r="L10" s="3">
+        <v>-9.9598999999999993E-2</v>
+      </c>
+      <c r="M10" s="3">
+        <v>0.43077900000000002</v>
+      </c>
+      <c r="N10" s="3">
+        <v>0.34834500000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0.26026300000000002</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.11131199999999999</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.26026300000000002</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0.32011299999999998</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0.31992999999999999</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0.20709</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0.24285399999999999</v>
+      </c>
+      <c r="J11" s="3">
+        <v>0.19302</v>
+      </c>
+      <c r="K11" s="3">
+        <v>1</v>
+      </c>
+      <c r="L11" s="3">
+        <v>7.5914999999999996E-2</v>
+      </c>
+      <c r="M11" s="3">
+        <v>0.410387</v>
+      </c>
+      <c r="N11" s="3">
+        <v>0.35066799999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0.36806100000000003</v>
+      </c>
+      <c r="C12" s="3">
+        <v>4.0870999999999998E-2</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.36954300000000001</v>
+      </c>
+      <c r="E12" s="3">
+        <v>4.5581000000000003E-2</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.211641</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0.25852999999999998</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0.32253500000000002</v>
+      </c>
+      <c r="I12" s="3">
+        <v>0.19620899999999999</v>
+      </c>
+      <c r="J12" s="3">
+        <v>-9.9598999999999993E-2</v>
+      </c>
+      <c r="K12" s="3">
+        <v>7.5914999999999996E-2</v>
+      </c>
+      <c r="L12" s="3">
+        <v>1</v>
+      </c>
+      <c r="M12" s="3">
+        <v>0.29969600000000002</v>
+      </c>
+      <c r="N12" s="3">
+        <v>0.115647</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="B13" s="3">
+        <v>0.58664099999999997</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.30540499999999998</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.61166500000000001</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.59738100000000005</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0.71648900000000004</v>
+      </c>
+      <c r="G13" s="3">
+        <v>0.74404800000000004</v>
+      </c>
+      <c r="H13" s="3">
+        <v>0.59240999999999999</v>
+      </c>
+      <c r="I13" s="3">
+        <v>0.473109</v>
+      </c>
+      <c r="J13" s="3">
+        <v>0.43077900000000002</v>
+      </c>
+      <c r="K13" s="3">
+        <v>0.410387</v>
+      </c>
+      <c r="L13" s="3">
+        <v>0.29969600000000002</v>
+      </c>
+      <c r="M13" s="3">
+        <v>1</v>
+      </c>
+      <c r="N13" s="3">
+        <v>0.795014</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="B14" s="3">
+        <v>0.46189999999999998</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.239118</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0.48731999999999998</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0.51170800000000005</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0.58902200000000005</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0.61249600000000004</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0.47600999999999999</v>
+      </c>
+      <c r="I14" s="3">
+        <v>0.35311399999999998</v>
+      </c>
+      <c r="J14" s="3">
+        <v>0.34834500000000002</v>
+      </c>
+      <c r="K14" s="3">
+        <v>0.35066799999999998</v>
+      </c>
+      <c r="L14" s="3">
+        <v>0.115647</v>
+      </c>
+      <c r="M14" s="3">
+        <v>0.795014</v>
+      </c>
+      <c r="N14" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>286</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:N14">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>0.7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B26"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" zoomScale="161" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="B1" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>211</v>
+      <c r="A2">
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>98</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>212</v>
+      <c r="A3">
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>182</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>213</v>
+      <c r="A4">
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>99</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>214</v>
+      <c r="A5">
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>100</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>215</v>
+      <c r="A6">
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>191</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>216</v>
+      <c r="A7">
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>101</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>217</v>
+      <c r="A8">
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>206</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>218</v>
+      <c r="A9">
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>102</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>219</v>
+      <c r="A10">
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>179</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>220</v>
+      <c r="A11">
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>103</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>221</v>
+      <c r="A12">
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>104</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>222</v>
+      <c r="A13">
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>203</v>
+        <v>143</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>223</v>
+      <c r="A14">
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>202</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>224</v>
+      <c r="A15">
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>207</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>225</v>
+      <c r="A16">
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>208</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>226</v>
+      <c r="A17">
+        <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>209</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>227</v>
+      <c r="A18">
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>104</v>
+        <v>145</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>228</v>
+      <c r="A19">
+        <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>183</v>
+        <v>146</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>229</v>
+      <c r="A20">
+        <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>105</v>
+        <v>147</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>230</v>
+      <c r="A21">
+        <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>189</v>
+        <v>148</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>231</v>
+      <c r="A22">
+        <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>106</v>
+        <v>149</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>232</v>
+      <c r="A23">
+        <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>107</v>
+        <v>150</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>233</v>
+      <c r="A24">
+        <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>186</v>
+        <v>151</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>234</v>
+      <c r="A25">
+        <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>185</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>235</v>
+      <c r="A26">
+        <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>236</v>
-      </c>
-      <c r="B27" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>237</v>
-      </c>
-      <c r="B28" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>238</v>
-      </c>
-      <c r="B29" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>239</v>
-      </c>
-      <c r="B30" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>240</v>
-      </c>
-      <c r="B31" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>241</v>
-      </c>
-      <c r="B32" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>242</v>
-      </c>
-      <c r="B33" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>243</v>
-      </c>
-      <c r="B34" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>244</v>
-      </c>
-      <c r="B35" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>245</v>
-      </c>
-      <c r="B36" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>246</v>
-      </c>
-      <c r="B37" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>247</v>
-      </c>
-      <c r="B38" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>248</v>
-      </c>
-      <c r="B39" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>249</v>
-      </c>
-      <c r="B40" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>250</v>
-      </c>
-      <c r="B41" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>251</v>
-      </c>
-      <c r="B42" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>252</v>
-      </c>
-      <c r="B43" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>253</v>
-      </c>
-      <c r="B44" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>254</v>
-      </c>
-      <c r="B45" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>255</v>
-      </c>
-      <c r="B46" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>256</v>
-      </c>
-      <c r="B47" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>257</v>
-      </c>
-      <c r="B48" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>258</v>
-      </c>
-      <c r="B49" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>259</v>
-      </c>
-      <c r="B50" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>260</v>
-      </c>
-      <c r="B51" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>261</v>
-      </c>
-      <c r="B52" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>262</v>
-      </c>
-      <c r="B53" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>263</v>
-      </c>
-      <c r="B54" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>264</v>
-      </c>
-      <c r="B55" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>265</v>
-      </c>
-      <c r="B56" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>266</v>
-      </c>
-      <c r="B57" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>267</v>
-      </c>
-      <c r="B58" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>210</v>
-      </c>
-      <c r="B59" t="s">
-        <v>205</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -1650,231 +3117,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B26"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>132</v>
-      </c>
-      <c r="B1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26" t="s">
-        <v>152</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2100,8 +3344,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2403,11 +3647,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -2530,8 +3774,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
@@ -2769,8 +4013,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2936,8 +4180,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>